<commit_message>
Finished ISS Orbit scenario error analysis
Closes issue #45
</commit_message>
<xml_diff>
--- a/Design and Notes/ISS_Scenario_Error_Analysis.xlsx
+++ b/Design and Notes/ISS_Scenario_Error_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\Gravity-Sandbox\Design and Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009B791-A82A-42E4-AC7A-87F56FB08820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8986DD1-2F85-4B93-8CDF-03AEBC52961E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="870" windowWidth="25230" windowHeight="20610" xr2:uid="{95A0EBFF-35AE-4473-B235-16AE549DD125}"/>
+    <workbookView xWindow="2685" yWindow="30" windowWidth="25230" windowHeight="20610" xr2:uid="{95A0EBFF-35AE-4473-B235-16AE549DD125}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>ISS Orbit Scenario - Analysis of approximation error in original algorithm</t>
   </si>
@@ -141,6 +141,24 @@
   </si>
   <si>
     <t>Cosine</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Error in One Step</t>
+  </si>
+  <si>
+    <t>Position Error</t>
+  </si>
+  <si>
+    <t>Velocity Error</t>
+  </si>
+  <si>
+    <t>Error Percentages</t>
   </si>
 </sst>
 </file>
@@ -148,7 +166,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -279,7 +297,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="4" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -299,6 +317,388 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>109171</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>65331</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D8CF7C-5065-42EF-AD28-6442B804EAC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5562600" y="5305425"/>
+          <a:ext cx="7491046" cy="6532806"/>
+          <a:chOff x="967154" y="344244"/>
+          <a:chExt cx="7491046" cy="6513756"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDCFFC31-E10E-41EB-83F8-36948FF89CFA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="967154" y="1881554"/>
+            <a:ext cx="756138" cy="1869831"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="en-US"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="10" name="Group 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DB74D61-4E7B-4798-94F3-057D0B795917}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1164104" y="344244"/>
+            <a:ext cx="7294096" cy="6513756"/>
+            <a:chOff x="1164104" y="344244"/>
+            <a:chExt cx="7294096" cy="6513756"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="Arc 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{952F31A0-5CB8-400F-8330-F739D9CD7874}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="1175826" y="344244"/>
+              <a:ext cx="7282374" cy="6513756"/>
+            </a:xfrm>
+            <a:prstGeom prst="arc">
+              <a:avLst>
+                <a:gd name="adj1" fmla="val 20062754"/>
+                <a:gd name="adj2" fmla="val 0"/>
+              </a:avLst>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="en-US"/>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1800" kern="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="12" name="Straight Connector 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32776712-915A-4306-9DAD-E8C2B8E15706}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="1164104" y="1957754"/>
+              <a:ext cx="464455" cy="1643369"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,15 +998,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6557784F-802C-4164-B937-0491A211CAAC}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -848,80 +1249,89 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <f>SQRT(B23*B23+C23*C23)</f>
+        <v>460.568411451869</v>
+      </c>
+      <c r="C27">
+        <f>ATAN(B23/C23)*(360/(2*PI()))</f>
+        <v>3.868388635371828</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>270</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <f>B6/60</f>
         <v>459.51907658440001</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <f>2 * PI() * B5</f>
         <v>42698.76805570646</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="9">
-        <f>B30/B31</f>
-        <v>1.0761881372898012E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="9">
+        <f>B31/B32</f>
+        <v>1.0761881372898012E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B33">
-        <f>B32*360</f>
+      <c r="B34">
+        <f>B33*360</f>
         <v>3.8742772942432842</v>
       </c>
-      <c r="C33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35">
-        <f>B29+B33</f>
-        <v>273.87427729424326</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="C34" t="s">
         <v>31</v>
       </c>
     </row>
@@ -930,67 +1340,235 @@
         <v>24</v>
       </c>
       <c r="B36">
-        <f>RADIANS(B35)</f>
+        <f>B30+B34</f>
+        <v>273.87427729424326</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <f>RADIANS(B36)</f>
         <v>4.7800078753044914</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <f>SIN(B36)</f>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f>SIN(B37)</f>
         <v>-0.99771471347816076</v>
       </c>
-      <c r="C39">
-        <f>COS(B36)</f>
+      <c r="C40">
+        <f>COS(B37)</f>
         <v>6.7567377551534399E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42">
-        <f>$B$5*B39</f>
-        <v>-6780.1898326778073</v>
-      </c>
-      <c r="C42">
-        <f>$B$5*C39</f>
-        <v>459.16897897451338</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43">
+        <f>$B$5*B40</f>
+        <v>-6780.1898326778073</v>
+      </c>
+      <c r="C43">
+        <f>$B$5*C40</f>
+        <v>459.16897897451338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>23</v>
       </c>
-      <c r="B43">
-        <f>$D$6*C39</f>
+      <c r="B44">
+        <f>$D$6*C40</f>
         <v>31.048498939710605</v>
       </c>
-      <c r="C43">
-        <f>-$D$6*B39</f>
+      <c r="C44">
+        <f>-$D$6*B40</f>
         <v>458.46894383215368</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47">
+        <f>SQRT(B44*B44+C44*C44)</f>
+        <v>459.51907658440001</v>
+      </c>
+      <c r="C47">
+        <f>ATAN(B44/C44)*(360/(2*PI()))</f>
+        <v>3.874277294243234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51">
+        <f>B24-B43</f>
+        <v>5.9187544093219913E-3</v>
+      </c>
+      <c r="C51">
+        <f>C24-C43</f>
+        <v>0.35009760988663174</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52">
+        <f>B23-B44</f>
+        <v>2.3673213494696199E-2</v>
+      </c>
+      <c r="C52">
+        <f>C23-C44</f>
+        <v>1.0501327522463271</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55">
+        <f>B27-B47</f>
+        <v>1.0493348674689855</v>
+      </c>
+      <c r="C55">
+        <f>C27-C47</f>
+        <v>-5.888658871405994E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="9">
+        <f>B51/B43</f>
+        <v>-8.7294818513723006E-7</v>
+      </c>
+      <c r="C60" s="9">
+        <f>C51/C43</f>
+        <v>7.6245919458349173E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="9">
+        <f>B52/B44</f>
+        <v>7.624591945866498E-4</v>
+      </c>
+      <c r="C61" s="9">
+        <f>C52/C44</f>
+        <v>2.2905210186511186E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" s="9">
+        <f>B55/B47</f>
+        <v>2.2835501743881438E-3</v>
+      </c>
+      <c r="C64" s="9">
+        <f>C55/C47</f>
+        <v>-1.5199373777803457E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>